<commit_message>
Confirmo cambios, remapeo de base de datos
</commit_message>
<xml_diff>
--- a/WebAPI/wwwroot/Plantillas/ReplicasLaboratorioExterno.xlsx
+++ b/WebAPI/wwwroot/Plantillas/ReplicasLaboratorioExterno.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>CLAVE SITIO</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>No. CARGA</t>
+  </si>
+  <si>
+    <t>NOMBRE(s) ARCHIVO EVIDENCIA</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -154,11 +157,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -173,6 +187,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -455,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,7 +499,7 @@
     <col min="17" max="18" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -536,6 +553,9 @@
       </c>
       <c r="R1" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>